<commit_message>
Added Playwright test pom test data and some comments
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -1,62 +1,423 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <bookViews>
+    <workbookView windowWidth="28800" windowHeight="11440"/>
+  </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>Peter Mac Anderson</t>
+  </si>
+  <si>
+    <t>Enabled</t>
+  </si>
+  <si>
+    <t>SonGoku</t>
+  </si>
+  <si>
+    <t>songoku102030</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="21">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -64,18 +425,312 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Link" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -395,61 +1050,66 @@
       </a:style>
     </a:lnDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultColWidth="7.94117647058824" defaultRowHeight="17.6" outlineLevelRow="3" outlineLevelCol="5"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>login</v>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
-      <c r="B1" t="str">
-        <v>Admin</v>
+      <c r="B1" t="s">
+        <v>1</v>
       </c>
-      <c r="C1" t="str">
-        <v>admin123</v>
+      <c r="C1" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Admin</v>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>1</v>
       </c>
-      <c r="B2" t="str">
-        <v>Peter Mac Anderson</v>
+      <c r="B2" t="s">
+        <v>3</v>
       </c>
-      <c r="C2" t="str">
-        <v>Enabled</v>
+      <c r="C2" t="s">
+        <v>4</v>
       </c>
-      <c r="D2" t="str">
-        <v>SonGoku</v>
+      <c r="D2" t="s">
+        <v>5</v>
       </c>
-      <c r="E2" t="str">
-        <v>songoku102030</v>
+      <c r="E2" t="s">
+        <v>6</v>
       </c>
-      <c r="F2" t="str">
-        <v>songoku102030</v>
+      <c r="F2" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v/>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="4">
-      <c r="B4" t="str">
-        <v/>
+    <row r="4" spans="2:2">
+      <c r="B4" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F4"/>
+    <ignoredError sqref="A1:F4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>